<commit_message>
more tests and coverage and better cryptography
</commit_message>
<xml_diff>
--- a/sample/test/simple_with_hidden_sheets.xlsx
+++ b/sample/test/simple_with_hidden_sheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\The Gang\exco\sample\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF18CC9E-D3FD-4CE9-A907-1F006B583E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F681C741-A3A6-41A5-A225-74801B8078DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -394,7 +394,7 @@
   <dimension ref="C3:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>